<commit_message>
Current best solution at 0.7757832711517303.
</commit_message>
<xml_diff>
--- a/task3_handout/gridsearch.xlsx
+++ b/task3_handout/gridsearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrysanderhagen/My Drive/ETH_Zurich/Studieren/2023HS/PAI/Projects/PAI_v2/task3_handout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996A85B5-8878-2F41-B6C9-3435292EF375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3536185A-3576-4F46-86F1-859C643CDF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{B0E64FD6-1876-9F40-944B-8DE816F7D2EE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>LAMBDA</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>0.6934390427509218</t>
+  </si>
+  <si>
+    <t>0.7757707945031895</t>
+  </si>
+  <si>
+    <t>NU_F</t>
+  </si>
+  <si>
+    <t>NU_V</t>
   </si>
 </sst>
 </file>
@@ -480,18 +489,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA04E2AF-F1FE-CE4D-B8EA-8C62138D642F}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,13 +512,19 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -518,11 +534,17 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -532,11 +554,17 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>100</v>
       </c>
@@ -546,11 +574,17 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1000</v>
       </c>
@@ -560,11 +594,17 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>10000</v>
       </c>
@@ -574,11 +614,17 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>100</v>
       </c>
@@ -588,11 +634,17 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>100</v>
       </c>
@@ -602,11 +654,17 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>100</v>
       </c>
@@ -616,11 +674,17 @@
       <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>100</v>
       </c>
@@ -630,11 +694,17 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>100</v>
       </c>
@@ -644,11 +714,17 @@
       <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -658,14 +734,20 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>100</v>
       </c>
@@ -675,14 +757,20 @@
       <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>100</v>
       </c>
@@ -692,14 +780,20 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E14" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>100</v>
       </c>
@@ -709,14 +803,20 @@
       <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>100</v>
       </c>
@@ -726,14 +826,20 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>100</v>
       </c>
@@ -743,14 +849,20 @@
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>100</v>
       </c>
@@ -760,14 +872,20 @@
       <c r="C18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>100</v>
       </c>
@@ -777,14 +895,20 @@
       <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>100</v>
       </c>
@@ -794,14 +918,20 @@
       <c r="C20" s="1">
         <v>10</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>100</v>
       </c>
@@ -811,14 +941,20 @@
       <c r="C21" s="1">
         <v>100</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>50</v>
       </c>
@@ -828,14 +964,20 @@
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>5</v>
       </c>
@@ -845,62 +987,110 @@
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>50</v>
+      </c>
+      <c r="B24" s="1">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F25">
+        <v>0.77578327115172996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>100</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="F26">
+        <v>0.77578323012968098</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>

</xml_diff>

<commit_message>
Tried different exploration parameters/ .
</commit_message>
<xml_diff>
--- a/task3_handout/gridsearch.xlsx
+++ b/task3_handout/gridsearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chrysanderhagen/My Drive/ETH_Zurich/Studieren/2023HS/PAI/Projects/PAI_v2/task3_handout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B2EA19-EEF1-0D44-B65F-AD7687B92B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7B9E1F-6AE0-2C41-9D0B-32CAFE533BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{B0E64FD6-1876-9F40-944B-8DE816F7D2EE}"/>
   </bookViews>
@@ -509,8 +509,8 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>